<commit_message>
diknas converted items phase1
</commit_message>
<xml_diff>
--- a/lib/tasks/diknascourses.xlsx
+++ b/lib/tasks/diknascourses.xlsx
@@ -24,14 +24,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>AGAMA</t>
   </si>
   <si>
-    <t>PKN</t>
-  </si>
-  <si>
     <t>BAHASA INDONESIA</t>
   </si>
   <si>
@@ -59,30 +56,15 @@
     <t>SOSIOLOGI</t>
   </si>
   <si>
-    <t>SASTRA</t>
-  </si>
-  <si>
-    <t>ANTROPOLOGI</t>
-  </si>
-  <si>
-    <t>BAHASA ASING</t>
-  </si>
-  <si>
     <t>SEJARAH</t>
   </si>
   <si>
     <t>SENI BUDAYA</t>
   </si>
   <si>
-    <t>PENJASORKES</t>
-  </si>
-  <si>
     <t>TIK</t>
   </si>
   <si>
-    <t>MUATAN LOKAL</t>
-  </si>
-  <si>
     <t>no</t>
   </si>
   <si>
@@ -90,6 +72,54 @@
   </si>
   <si>
     <t>notes</t>
+  </si>
+  <si>
+    <t>PENJASORKES BOYS</t>
+  </si>
+  <si>
+    <t>PENJASORKES GIRLS</t>
+  </si>
+  <si>
+    <t>ART</t>
+  </si>
+  <si>
+    <t>BIOLOGI INTERNATIONAL</t>
+  </si>
+  <si>
+    <t>DEBAT</t>
+  </si>
+  <si>
+    <t>FISIKA INTERNATIONAL</t>
+  </si>
+  <si>
+    <t>LITERATUR</t>
+  </si>
+  <si>
+    <t>LITERATUR INDONESIA</t>
+  </si>
+  <si>
+    <t>MATEMATIKASS</t>
+  </si>
+  <si>
+    <t>SERVICE ELECTIVE</t>
+  </si>
+  <si>
+    <t>UN EKONOMI</t>
+  </si>
+  <si>
+    <t>UN MATEMATIKASS</t>
+  </si>
+  <si>
+    <t>UN MATEMATIKA</t>
+  </si>
+  <si>
+    <t>WALI KELAS</t>
+  </si>
+  <si>
+    <t>ENGLISH TUTORING</t>
+  </si>
+  <si>
+    <t>SPANYOL</t>
   </si>
 </sst>
 </file>
@@ -432,26 +462,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:C30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="F1" sqref="F1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -464,105 +495,105 @@
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="2" t="s">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="C3" s="2"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C4" s="2"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C5" s="2"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="2" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C6" s="2"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="2" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="C7" s="2"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="2" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="C8" s="2"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C9" s="2"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="2" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C10" s="2"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="2" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="C11" s="2"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C12" s="2"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="2" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C13" s="2"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="2" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="C14" s="2"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="2" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="C15" s="2"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="2" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="C16" s="2"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="2" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="C17" s="2"/>
     </row>
@@ -583,9 +614,59 @@
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
       <c r="B20" s="2" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="C20" s="2"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>31</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>